<commit_message>
Retoques en la web!
</commit_message>
<xml_diff>
--- a/docs/Diarios.xlsx
+++ b/docs/Diarios.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="diarios" sheetId="1" r:id="rId1"/>
     <sheet name="costos-appengine" sheetId="2" r:id="rId2"/>
     <sheet name="Prospects" sheetId="3" r:id="rId3"/>
     <sheet name="Listado" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">diarios!$E$1:$E$180</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="1256">
   <si>
     <t>nombre</t>
   </si>
@@ -3884,6 +3885,90 @@
   <si>
     <t>Lista completa: http://www.prensaescrita.com/america/argentina.php</t>
   </si>
+  <si>
+    <t>wgoni@hotmail.com</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Claudio</t>
+  </si>
+  <si>
+    <t>indioluque@gmail.com</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>nloyarte@ellitoral.com</t>
+  </si>
+  <si>
+    <t>domar@ellitoral.com</t>
+  </si>
+  <si>
+    <t>Nicolás</t>
+  </si>
+  <si>
+    <t>Darío</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Rosario</t>
+  </si>
+  <si>
+    <t>Salta / Jujuy</t>
+  </si>
+  <si>
+    <t>cbazan@diaadia.com.ar</t>
+  </si>
+  <si>
+    <t>Cecilia</t>
+  </si>
+  <si>
+    <t>Día a día</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ipisani@rionegro.com.ar </t>
+  </si>
+  <si>
+    <t>Italo</t>
+  </si>
+  <si>
+    <t>hpalavecino@lacapitalmdq.com</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Mar del Plata</t>
+  </si>
+  <si>
+    <t>dcapristo@lanuevaprovincia.com.ar</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Bahia Blanca</t>
+  </si>
+  <si>
+    <t>caluromero@ellitoral.com.ar</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>sbravo@ellitoral.com.ar</t>
+  </si>
+  <si>
+    <t>Sebastián</t>
+  </si>
 </sst>
 </file>
 
@@ -3893,7 +3978,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000000_);[Red]\(&quot;$&quot;#,##0.000000\)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4085,6 +4170,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -4510,7 +4602,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4551,6 +4643,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -16154,7 +16249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -16760,4 +16855,224 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="19"/>
+    <col min="3" max="3" width="20" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="18" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="20" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A10" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+</worksheet>
 </file>
</xml_diff>